<commit_message>
changes to add ss_id and pmid to all new items and avoid duplicate bibkeys
</commit_message>
<xml_diff>
--- a/scripts/script_data/manual_check_20231018.xlsx
+++ b/scripts/script_data/manual_check_20231018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://radboudumc.sharepoint.com/sites/teamsdiagradiologieennucleairegeneeskunde-Webteam-private/Gedeelde documenten/Webteam-private/Literature - manual check/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keeli\nov23\repos\Literature\scripts\script_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="605" documentId="13_ncr:1_{D6F274B8-1CC9-494C-85A4-7E6E562CBDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80765411-A518-428E-AE54-D261EF730A1A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CCB134-9585-4D55-856D-0208EDBCE56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4888" uniqueCount="2611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4898" uniqueCount="2616">
   <si>
     <t>bibkey</t>
   </si>
@@ -7872,13 +7870,28 @@
   </si>
   <si>
     <t>C. Marrocco and A. Bria and Valerio Di Sano and L. Borges and B. Savelli and M. Molinara and J. Mordang and N. Karssemeijer and F. Tortorella</t>
+  </si>
+  <si>
+    <t>10.1016/j.tcs.2018.10.026</t>
+  </si>
+  <si>
+    <t>(requested by Stan)</t>
+  </si>
+  <si>
+    <t>10.1186/s41747-023-00372-7</t>
+  </si>
+  <si>
+    <t>fde118f6324d87e79811f01522e106e64237bec2</t>
+  </si>
+  <si>
+    <t>03a7b0c8377b4cfd5bd37215d644d31033b7ae23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7917,6 +7930,29 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -7964,7 +8000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -7982,6 +8018,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8285,26 +8324,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W284"/>
+  <dimension ref="A1:X284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O80" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="V97" sqref="V97"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B271" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
+      <selection pane="bottomRight" activeCell="A285" sqref="A285"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="47.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="20" max="20" width="43.42578125" customWidth="1"/>
+    <col min="2" max="2" width="47.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" customWidth="1"/>
+    <col min="8" max="8" width="27.26953125" customWidth="1"/>
+    <col min="20" max="20" width="43.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8372,7 +8411,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -8431,7 +8470,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -8490,7 +8529,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -8546,7 +8585,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -8602,7 +8641,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -8661,7 +8700,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -8714,7 +8753,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -8779,7 +8818,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -8838,7 +8877,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>130</v>
       </c>
@@ -8897,7 +8936,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -8953,7 +8992,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -9015,7 +9054,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>162</v>
       </c>
@@ -9074,7 +9113,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>173</v>
       </c>
@@ -9133,7 +9172,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>183</v>
       </c>
@@ -9198,7 +9237,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>197</v>
       </c>
@@ -9257,7 +9296,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>207</v>
       </c>
@@ -9319,7 +9358,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>221</v>
       </c>
@@ -9384,7 +9423,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>233</v>
       </c>
@@ -9446,7 +9485,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>244</v>
       </c>
@@ -9508,7 +9547,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="14.1" customHeight="1">
+    <row r="21" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>258</v>
       </c>
@@ -9567,7 +9606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>267</v>
       </c>
@@ -9629,7 +9668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>280</v>
       </c>
@@ -9688,7 +9727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>290</v>
       </c>
@@ -9747,7 +9786,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>300</v>
       </c>
@@ -9812,7 +9851,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>313</v>
       </c>
@@ -9868,7 +9907,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>322</v>
       </c>
@@ -9921,7 +9960,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>332</v>
       </c>
@@ -9980,7 +10019,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>337</v>
       </c>
@@ -10042,7 +10081,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>347</v>
       </c>
@@ -10098,7 +10137,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>353</v>
       </c>
@@ -10163,7 +10202,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>365</v>
       </c>
@@ -10225,7 +10264,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>379</v>
       </c>
@@ -10287,7 +10326,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>388</v>
       </c>
@@ -10337,7 +10376,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>394</v>
       </c>
@@ -10399,7 +10438,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>404</v>
       </c>
@@ -10452,7 +10491,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>412</v>
       </c>
@@ -10511,7 +10550,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>422</v>
       </c>
@@ -10570,7 +10609,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="30.75">
+    <row r="39" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>433</v>
       </c>
@@ -10632,7 +10671,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>442</v>
       </c>
@@ -10697,7 +10736,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>454</v>
       </c>
@@ -10756,7 +10795,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="30.75">
+    <row r="42" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>464</v>
       </c>
@@ -10818,7 +10857,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>474</v>
       </c>
@@ -10883,7 +10922,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>486</v>
       </c>
@@ -10948,7 +10987,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>497</v>
       </c>
@@ -11013,7 +11052,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>509</v>
       </c>
@@ -11072,7 +11111,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>519</v>
       </c>
@@ -11131,7 +11170,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>527</v>
       </c>
@@ -11187,7 +11226,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>536</v>
       </c>
@@ -11252,7 +11291,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>544</v>
       </c>
@@ -11308,7 +11347,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>553</v>
       </c>
@@ -11367,7 +11406,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>562</v>
       </c>
@@ -11432,7 +11471,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>576</v>
       </c>
@@ -11491,7 +11530,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>585</v>
       </c>
@@ -11550,7 +11589,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>595</v>
       </c>
@@ -11612,7 +11651,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>606</v>
       </c>
@@ -11671,7 +11710,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="57" spans="1:23">
+    <row r="57" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>412</v>
       </c>
@@ -11736,7 +11775,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>622</v>
       </c>
@@ -11801,7 +11840,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>633</v>
       </c>
@@ -11860,7 +11899,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>643</v>
       </c>
@@ -11919,7 +11958,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>653</v>
       </c>
@@ -11972,7 +12011,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>663</v>
       </c>
@@ -12037,7 +12076,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>673</v>
       </c>
@@ -12096,7 +12135,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>683</v>
       </c>
@@ -12158,7 +12197,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>693</v>
       </c>
@@ -12205,7 +12244,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>433</v>
       </c>
@@ -12267,7 +12306,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>706</v>
       </c>
@@ -12326,7 +12365,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>716</v>
       </c>
@@ -12391,7 +12430,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>725</v>
       </c>
@@ -12444,7 +12483,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>733</v>
       </c>
@@ -12509,7 +12548,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>744</v>
       </c>
@@ -12568,7 +12607,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>754</v>
       </c>
@@ -12633,7 +12672,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>766</v>
       </c>
@@ -12695,7 +12734,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>776</v>
       </c>
@@ -12748,7 +12787,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>783</v>
       </c>
@@ -12807,7 +12846,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="76" spans="1:23">
+    <row r="76" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>793</v>
       </c>
@@ -12872,7 +12911,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="30.75">
+    <row r="77" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>806</v>
       </c>
@@ -12931,7 +12970,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="78" spans="1:23">
+    <row r="78" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>544</v>
       </c>
@@ -12984,7 +13023,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="79" spans="1:23">
+    <row r="79" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>819</v>
       </c>
@@ -13049,7 +13088,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="80" spans="1:23">
+    <row r="80" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>830</v>
       </c>
@@ -13108,7 +13147,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="81" spans="1:22">
+    <row r="81" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>595</v>
       </c>
@@ -13173,7 +13212,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="82" spans="1:22">
+    <row r="82" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>776</v>
       </c>
@@ -13229,7 +13268,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="83" spans="1:22">
+    <row r="83" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>850</v>
       </c>
@@ -13294,7 +13333,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="84" spans="1:22">
+    <row r="84" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>861</v>
       </c>
@@ -13353,7 +13392,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="85" spans="1:22">
+    <row r="85" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>871</v>
       </c>
@@ -13415,7 +13454,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="86" spans="1:22">
+    <row r="86" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>882</v>
       </c>
@@ -13477,7 +13516,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="87" spans="1:22">
+    <row r="87" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>893</v>
       </c>
@@ -13536,7 +13575,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="88" spans="1:22">
+    <row r="88" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>903</v>
       </c>
@@ -13601,7 +13640,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="89" spans="1:22">
+    <row r="89" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>915</v>
       </c>
@@ -13663,7 +13702,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="90" spans="1:22">
+    <row r="90" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>733</v>
       </c>
@@ -13728,7 +13767,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="91" spans="1:22">
+    <row r="91" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>932</v>
       </c>
@@ -13781,7 +13820,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="92" spans="1:22">
+    <row r="92" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>937</v>
       </c>
@@ -13846,7 +13885,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="93" spans="1:22">
+    <row r="93" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>947</v>
       </c>
@@ -13899,7 +13938,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="94" spans="1:22">
+    <row r="94" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>955</v>
       </c>
@@ -13955,7 +13994,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="95" spans="1:22">
+    <row r="95" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>964</v>
       </c>
@@ -14014,7 +14053,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="96" spans="1:22">
+    <row r="96" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>519</v>
       </c>
@@ -14067,7 +14106,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="97" spans="1:22">
+    <row r="97" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>978</v>
       </c>
@@ -14126,7 +14165,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="98" spans="1:22">
+    <row r="98" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>987</v>
       </c>
@@ -14188,7 +14227,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="99" spans="1:22">
+    <row r="99" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>997</v>
       </c>
@@ -14241,7 +14280,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="100" spans="1:22">
+    <row r="100" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>1004</v>
       </c>
@@ -14306,7 +14345,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="101" spans="1:22">
+    <row r="101" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>1012</v>
       </c>
@@ -14365,7 +14404,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="102" spans="1:22">
+    <row r="102" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>1021</v>
       </c>
@@ -14421,7 +14460,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="103" spans="1:22">
+    <row r="103" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>1030</v>
       </c>
@@ -14480,7 +14519,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="104" spans="1:22">
+    <row r="104" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>1040</v>
       </c>
@@ -14542,7 +14581,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="105" spans="1:22">
+    <row r="105" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>1050</v>
       </c>
@@ -14604,7 +14643,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="106" spans="1:22">
+    <row r="106" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>1059</v>
       </c>
@@ -14669,7 +14708,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="107" spans="1:22">
+    <row r="107" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>1069</v>
       </c>
@@ -14731,7 +14770,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="108" spans="1:22">
+    <row r="108" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>1080</v>
       </c>
@@ -14784,7 +14823,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="109" spans="1:22">
+    <row r="109" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>1087</v>
       </c>
@@ -14843,7 +14882,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="110" spans="1:22">
+    <row r="110" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>322</v>
       </c>
@@ -14902,7 +14941,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="111" spans="1:22">
+    <row r="111" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>783</v>
       </c>
@@ -14961,7 +15000,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="112" spans="1:22">
+    <row r="112" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>1110</v>
       </c>
@@ -15020,7 +15059,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="113" spans="1:22">
+    <row r="113" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>1119</v>
       </c>
@@ -15076,7 +15115,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="114" spans="1:22">
+    <row r="114" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>1128</v>
       </c>
@@ -15135,7 +15174,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="115" spans="1:22">
+    <row r="115" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>1137</v>
       </c>
@@ -15191,7 +15230,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="116" spans="1:22">
+    <row r="116" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>754</v>
       </c>
@@ -15256,7 +15295,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="117" spans="1:22">
+    <row r="117" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>1151</v>
       </c>
@@ -15309,7 +15348,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="118" spans="1:22">
+    <row r="118" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>1159</v>
       </c>
@@ -15374,7 +15413,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="119" spans="1:22">
+    <row r="119" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>1171</v>
       </c>
@@ -15430,7 +15469,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="120" spans="1:22">
+    <row r="120" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>1181</v>
       </c>
@@ -15489,7 +15528,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="121" spans="1:22">
+    <row r="121" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>1191</v>
       </c>
@@ -15554,7 +15593,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="122" spans="1:22">
+    <row r="122" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>1202</v>
       </c>
@@ -15619,7 +15658,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="123" spans="1:22">
+    <row r="123" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>1214</v>
       </c>
@@ -15681,7 +15720,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="124" spans="1:22">
+    <row r="124" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>1223</v>
       </c>
@@ -15746,7 +15785,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="125" spans="1:22">
+    <row r="125" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>1235</v>
       </c>
@@ -15808,7 +15847,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="126" spans="1:22">
+    <row r="126" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>1243</v>
       </c>
@@ -15861,7 +15900,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="127" spans="1:22">
+    <row r="127" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>1249</v>
       </c>
@@ -15920,7 +15959,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="128" spans="1:22">
+    <row r="128" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>1259</v>
       </c>
@@ -15979,7 +16018,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="129" spans="1:22">
+    <row r="129" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>1269</v>
       </c>
@@ -16044,7 +16083,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="130" spans="1:22">
+    <row r="130" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>1279</v>
       </c>
@@ -16100,7 +16139,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="131" spans="1:22">
+    <row r="131" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>22</v>
       </c>
@@ -16159,7 +16198,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="132" spans="1:22">
+    <row r="132" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>1294</v>
       </c>
@@ -16221,7 +16260,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="133" spans="1:22">
+    <row r="133" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>207</v>
       </c>
@@ -16283,7 +16322,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="134" spans="1:22">
+    <row r="134" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>1308</v>
       </c>
@@ -16348,7 +16387,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="135" spans="1:22">
+    <row r="135" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>871</v>
       </c>
@@ -16413,7 +16452,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="136" spans="1:22">
+    <row r="136" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>1110</v>
       </c>
@@ -16475,7 +16514,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="137" spans="1:22">
+    <row r="137" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>1327</v>
       </c>
@@ -16534,7 +16573,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="138" spans="1:22">
+    <row r="138" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>1336</v>
       </c>
@@ -16599,7 +16638,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="139" spans="1:22">
+    <row r="139" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>1347</v>
       </c>
@@ -16658,7 +16697,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="140" spans="1:22">
+    <row r="140" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>1358</v>
       </c>
@@ -16717,7 +16756,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="141" spans="1:22">
+    <row r="141" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>1367</v>
       </c>
@@ -16782,7 +16821,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="142" spans="1:22">
+    <row r="142" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>1379</v>
       </c>
@@ -16838,7 +16877,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="143" spans="1:22">
+    <row r="143" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>1388</v>
       </c>
@@ -16897,7 +16936,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="144" spans="1:22">
+    <row r="144" spans="1:22" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>1397</v>
       </c>
@@ -16962,7 +17001,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="145" spans="1:23">
+    <row r="145" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>1409</v>
       </c>
@@ -17027,7 +17066,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="146" spans="1:23">
+    <row r="146" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>1420</v>
       </c>
@@ -17092,7 +17131,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="147" spans="1:23">
+    <row r="147" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>1432</v>
       </c>
@@ -17146,7 +17185,7 @@
       </c>
       <c r="V147" s="3"/>
     </row>
-    <row r="148" spans="1:23">
+    <row r="148" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>1440</v>
       </c>
@@ -17212,7 +17251,7 @@
       </c>
       <c r="V148" s="3"/>
     </row>
-    <row r="149" spans="1:23">
+    <row r="149" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>1451</v>
       </c>
@@ -17278,7 +17317,7 @@
       </c>
       <c r="V149" s="3"/>
     </row>
-    <row r="150" spans="1:23">
+    <row r="150" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>1462</v>
       </c>
@@ -17344,7 +17383,7 @@
       </c>
       <c r="V150" s="3"/>
     </row>
-    <row r="151" spans="1:23">
+    <row r="151" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>1473</v>
       </c>
@@ -17410,7 +17449,7 @@
       </c>
       <c r="V151" s="3"/>
     </row>
-    <row r="152" spans="1:23">
+    <row r="152" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>337</v>
       </c>
@@ -17478,7 +17517,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="153" spans="1:23">
+    <row r="153" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>1491</v>
       </c>
@@ -17540,7 +17579,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="154" spans="1:23">
+    <row r="154" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>1500</v>
       </c>
@@ -17600,7 +17639,7 @@
       </c>
       <c r="V154" s="3"/>
     </row>
-    <row r="155" spans="1:23">
+    <row r="155" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>1509</v>
       </c>
@@ -17663,7 +17702,7 @@
       </c>
       <c r="V155" s="3"/>
     </row>
-    <row r="156" spans="1:23">
+    <row r="156" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>1518</v>
       </c>
@@ -17729,7 +17768,7 @@
       </c>
       <c r="V156" s="3"/>
     </row>
-    <row r="157" spans="1:23">
+    <row r="157" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>1530</v>
       </c>
@@ -17789,7 +17828,7 @@
       </c>
       <c r="V157" s="3"/>
     </row>
-    <row r="158" spans="1:23">
+    <row r="158" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>1540</v>
       </c>
@@ -17855,7 +17894,7 @@
       </c>
       <c r="V158" s="3"/>
     </row>
-    <row r="159" spans="1:23">
+    <row r="159" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>1451</v>
       </c>
@@ -17917,7 +17956,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="160" spans="1:23">
+    <row r="160" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>733</v>
       </c>
@@ -17983,7 +18022,7 @@
       </c>
       <c r="V160" s="3"/>
     </row>
-    <row r="161" spans="1:23">
+    <row r="161" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>1560</v>
       </c>
@@ -18049,7 +18088,7 @@
       </c>
       <c r="V161" s="3"/>
     </row>
-    <row r="162" spans="1:23">
+    <row r="162" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>1570</v>
       </c>
@@ -18115,7 +18154,7 @@
       </c>
       <c r="V162" s="3"/>
     </row>
-    <row r="163" spans="1:23">
+    <row r="163" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>1579</v>
       </c>
@@ -18178,7 +18217,7 @@
       </c>
       <c r="V163" s="3"/>
     </row>
-    <row r="164" spans="1:23">
+    <row r="164" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>1590</v>
       </c>
@@ -18232,7 +18271,7 @@
       </c>
       <c r="V164" s="3"/>
     </row>
-    <row r="165" spans="1:23">
+    <row r="165" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>1597</v>
       </c>
@@ -18294,7 +18333,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="166" spans="1:23">
+    <row r="166" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>1606</v>
       </c>
@@ -18357,7 +18396,7 @@
       </c>
       <c r="V166" s="3"/>
     </row>
-    <row r="167" spans="1:23">
+    <row r="167" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>1615</v>
       </c>
@@ -18413,7 +18452,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="168" spans="1:23">
+    <row r="168" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>509</v>
       </c>
@@ -18473,7 +18512,7 @@
       </c>
       <c r="V168" s="3"/>
     </row>
-    <row r="169" spans="1:23">
+    <row r="169" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>1629</v>
       </c>
@@ -18532,7 +18571,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="170" spans="1:23">
+    <row r="170" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>1638</v>
       </c>
@@ -18589,7 +18628,7 @@
       </c>
       <c r="V170" s="3"/>
     </row>
-    <row r="171" spans="1:23">
+    <row r="171" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>1647</v>
       </c>
@@ -18651,7 +18690,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="172" spans="1:23">
+    <row r="172" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>1657</v>
       </c>
@@ -18713,7 +18752,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="173" spans="1:23">
+    <row r="173" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>1658</v>
       </c>
@@ -18770,7 +18809,7 @@
       </c>
       <c r="V173" s="3"/>
     </row>
-    <row r="174" spans="1:23">
+    <row r="174" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>1667</v>
       </c>
@@ -18835,7 +18874,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="175" spans="1:23">
+    <row r="175" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>1676</v>
       </c>
@@ -18901,7 +18940,7 @@
       </c>
       <c r="V175" s="3"/>
     </row>
-    <row r="176" spans="1:23">
+    <row r="176" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>1688</v>
       </c>
@@ -18961,7 +19000,7 @@
       </c>
       <c r="V176" s="3"/>
     </row>
-    <row r="177" spans="1:23">
+    <row r="177" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>1597</v>
       </c>
@@ -19026,7 +19065,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="178" spans="1:23">
+    <row r="178" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>1702</v>
       </c>
@@ -19088,7 +19127,7 @@
         <v>1712</v>
       </c>
     </row>
-    <row r="179" spans="1:23">
+    <row r="179" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>1713</v>
       </c>
@@ -19154,7 +19193,7 @@
       </c>
       <c r="V179" s="3"/>
     </row>
-    <row r="180" spans="1:23">
+    <row r="180" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>1724</v>
       </c>
@@ -19222,7 +19261,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="181" spans="1:23">
+    <row r="181" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>1737</v>
       </c>
@@ -19284,7 +19323,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="182" spans="1:23">
+    <row r="182" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>1746</v>
       </c>
@@ -19346,7 +19385,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="183" spans="1:23">
+    <row r="183" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>1756</v>
       </c>
@@ -19403,7 +19442,7 @@
       </c>
       <c r="V183" s="3"/>
     </row>
-    <row r="184" spans="1:23">
+    <row r="184" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>1763</v>
       </c>
@@ -19457,7 +19496,7 @@
       </c>
       <c r="V184" s="3"/>
     </row>
-    <row r="185" spans="1:23">
+    <row r="185" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>1766</v>
       </c>
@@ -19514,7 +19553,7 @@
       </c>
       <c r="V185" s="3"/>
     </row>
-    <row r="186" spans="1:23">
+    <row r="186" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>1775</v>
       </c>
@@ -19574,7 +19613,7 @@
       </c>
       <c r="V186" s="3"/>
     </row>
-    <row r="187" spans="1:23">
+    <row r="187" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>1784</v>
       </c>
@@ -19634,7 +19673,7 @@
       </c>
       <c r="V187" s="3"/>
     </row>
-    <row r="188" spans="1:23">
+    <row r="188" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>1793</v>
       </c>
@@ -19697,7 +19736,7 @@
       </c>
       <c r="V188" s="3"/>
     </row>
-    <row r="189" spans="1:23">
+    <row r="189" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>1805</v>
       </c>
@@ -19760,7 +19799,7 @@
       </c>
       <c r="V189" s="3"/>
     </row>
-    <row r="190" spans="1:23">
+    <row r="190" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>1815</v>
       </c>
@@ -19826,7 +19865,7 @@
       </c>
       <c r="V190" s="3"/>
     </row>
-    <row r="191" spans="1:23">
+    <row r="191" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>1825</v>
       </c>
@@ -19886,7 +19925,7 @@
       </c>
       <c r="V191" s="3"/>
     </row>
-    <row r="192" spans="1:23">
+    <row r="192" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>1834</v>
       </c>
@@ -19940,7 +19979,7 @@
       </c>
       <c r="V192" s="3"/>
     </row>
-    <row r="193" spans="1:23">
+    <row r="193" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>1841</v>
       </c>
@@ -20006,7 +20045,7 @@
       </c>
       <c r="V193" s="3"/>
     </row>
-    <row r="194" spans="1:23">
+    <row r="194" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>1851</v>
       </c>
@@ -20060,7 +20099,7 @@
       </c>
       <c r="V194" s="3"/>
     </row>
-    <row r="195" spans="1:23">
+    <row r="195" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>663</v>
       </c>
@@ -20126,7 +20165,7 @@
       </c>
       <c r="V195" s="3"/>
     </row>
-    <row r="196" spans="1:23">
+    <row r="196" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>1865</v>
       </c>
@@ -20189,7 +20228,7 @@
       </c>
       <c r="V196" s="3"/>
     </row>
-    <row r="197" spans="1:23">
+    <row r="197" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>1874</v>
       </c>
@@ -20246,7 +20285,7 @@
       </c>
       <c r="V197" s="3"/>
     </row>
-    <row r="198" spans="1:23">
+    <row r="198" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>1881</v>
       </c>
@@ -20312,7 +20351,7 @@
       </c>
       <c r="V198" s="3"/>
     </row>
-    <row r="199" spans="1:23">
+    <row r="199" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>509</v>
       </c>
@@ -20369,7 +20408,7 @@
       </c>
       <c r="V199" s="3"/>
     </row>
-    <row r="200" spans="1:23">
+    <row r="200" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>1898</v>
       </c>
@@ -20429,7 +20468,7 @@
       </c>
       <c r="V200" s="3"/>
     </row>
-    <row r="201" spans="1:23">
+    <row r="201" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>1908</v>
       </c>
@@ -20485,7 +20524,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="202" spans="1:23">
+    <row r="202" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>1914</v>
       </c>
@@ -20551,7 +20590,7 @@
       </c>
       <c r="V202" s="3"/>
     </row>
-    <row r="203" spans="1:23">
+    <row r="203" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>1925</v>
       </c>
@@ -20616,7 +20655,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="204" spans="1:23">
+    <row r="204" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>1936</v>
       </c>
@@ -20676,7 +20715,7 @@
       </c>
       <c r="V204" s="3"/>
     </row>
-    <row r="205" spans="1:23">
+    <row r="205" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>1945</v>
       </c>
@@ -20739,7 +20778,7 @@
       </c>
       <c r="V205" s="3"/>
     </row>
-    <row r="206" spans="1:23">
+    <row r="206" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>1956</v>
       </c>
@@ -20798,7 +20837,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="207" spans="1:23">
+    <row r="207" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>1965</v>
       </c>
@@ -20858,7 +20897,7 @@
       </c>
       <c r="V207" s="3"/>
     </row>
-    <row r="208" spans="1:23">
+    <row r="208" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>1975</v>
       </c>
@@ -20924,7 +20963,7 @@
       </c>
       <c r="V208" s="3"/>
     </row>
-    <row r="209" spans="1:23">
+    <row r="209" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>1986</v>
       </c>
@@ -20986,7 +21025,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="210" spans="1:23">
+    <row r="210" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>1997</v>
       </c>
@@ -21051,7 +21090,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="211" spans="1:23">
+    <row r="211" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>2007</v>
       </c>
@@ -21116,7 +21155,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="212" spans="1:23">
+    <row r="212" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>2018</v>
       </c>
@@ -21175,7 +21214,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="213" spans="1:23">
+    <row r="213" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>2028</v>
       </c>
@@ -21237,7 +21276,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="214" spans="1:23">
+    <row r="214" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>2037</v>
       </c>
@@ -21294,7 +21333,7 @@
       </c>
       <c r="V214" s="3"/>
     </row>
-    <row r="215" spans="1:23">
+    <row r="215" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>2045</v>
       </c>
@@ -21354,7 +21393,7 @@
       </c>
       <c r="V215" s="3"/>
     </row>
-    <row r="216" spans="1:23">
+    <row r="216" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>2055</v>
       </c>
@@ -21414,7 +21453,7 @@
       </c>
       <c r="V216" s="3"/>
     </row>
-    <row r="217" spans="1:23">
+    <row r="217" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>2065</v>
       </c>
@@ -21477,7 +21516,7 @@
       </c>
       <c r="V217" s="3"/>
     </row>
-    <row r="218" spans="1:23">
+    <row r="218" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>2074</v>
       </c>
@@ -21534,7 +21573,7 @@
       </c>
       <c r="V218" s="3"/>
     </row>
-    <row r="219" spans="1:23">
+    <row r="219" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>733</v>
       </c>
@@ -21600,7 +21639,7 @@
       </c>
       <c r="V219" s="3"/>
     </row>
-    <row r="220" spans="1:23">
+    <row r="220" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>1784</v>
       </c>
@@ -21663,7 +21702,7 @@
       </c>
       <c r="V220" s="3"/>
     </row>
-    <row r="221" spans="1:23">
+    <row r="221" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>2094</v>
       </c>
@@ -21723,7 +21762,7 @@
       </c>
       <c r="V221" s="3"/>
     </row>
-    <row r="222" spans="1:23">
+    <row r="222" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>2104</v>
       </c>
@@ -21791,7 +21830,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="223" spans="1:23">
+    <row r="223" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>2117</v>
       </c>
@@ -21847,7 +21886,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="224" spans="1:23">
+    <row r="224" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>2127</v>
       </c>
@@ -21913,7 +21952,7 @@
       </c>
       <c r="V224" s="3"/>
     </row>
-    <row r="225" spans="1:23">
+    <row r="225" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>2138</v>
       </c>
@@ -21970,7 +22009,7 @@
       </c>
       <c r="V225" s="3"/>
     </row>
-    <row r="226" spans="1:23">
+    <row r="226" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>2146</v>
       </c>
@@ -22029,7 +22068,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="227" spans="1:23">
+    <row r="227" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>2153</v>
       </c>
@@ -22082,7 +22121,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="228" spans="1:23">
+    <row r="228" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>2161</v>
       </c>
@@ -22145,7 +22184,7 @@
       </c>
       <c r="V228" s="3"/>
     </row>
-    <row r="229" spans="1:23">
+    <row r="229" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>2171</v>
       </c>
@@ -22211,7 +22250,7 @@
       </c>
       <c r="V229" s="3"/>
     </row>
-    <row r="230" spans="1:23">
+    <row r="230" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>497</v>
       </c>
@@ -22267,7 +22306,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="231" spans="1:23">
+    <row r="231" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>2184</v>
       </c>
@@ -22329,7 +22368,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="232" spans="1:23">
+    <row r="232" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>2194</v>
       </c>
@@ -22392,7 +22431,7 @@
       </c>
       <c r="V232" s="3"/>
     </row>
-    <row r="233" spans="1:23">
+    <row r="233" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>2205</v>
       </c>
@@ -22458,7 +22497,7 @@
       </c>
       <c r="V233" s="3"/>
     </row>
-    <row r="234" spans="1:23">
+    <row r="234" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>2215</v>
       </c>
@@ -22518,7 +22557,7 @@
       </c>
       <c r="V234" s="3"/>
     </row>
-    <row r="235" spans="1:23">
+    <row r="235" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>2225</v>
       </c>
@@ -22578,7 +22617,7 @@
       </c>
       <c r="V235" s="3"/>
     </row>
-    <row r="236" spans="1:23">
+    <row r="236" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>2235</v>
       </c>
@@ -22638,7 +22677,7 @@
       </c>
       <c r="V236" s="3"/>
     </row>
-    <row r="237" spans="1:23">
+    <row r="237" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>2245</v>
       </c>
@@ -22701,7 +22740,7 @@
       </c>
       <c r="V237" s="3"/>
     </row>
-    <row r="238" spans="1:23">
+    <row r="238" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>2255</v>
       </c>
@@ -22763,7 +22802,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="239" spans="1:23">
+    <row r="239" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>1793</v>
       </c>
@@ -22826,7 +22865,7 @@
       </c>
       <c r="V239" s="3"/>
     </row>
-    <row r="240" spans="1:23">
+    <row r="240" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>2271</v>
       </c>
@@ -22892,7 +22931,7 @@
       </c>
       <c r="V240" s="3"/>
     </row>
-    <row r="241" spans="1:23">
+    <row r="241" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>2279</v>
       </c>
@@ -22955,7 +22994,7 @@
       </c>
       <c r="V241" s="3"/>
     </row>
-    <row r="242" spans="1:23">
+    <row r="242" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>2007</v>
       </c>
@@ -23017,7 +23056,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="243" spans="1:23">
+    <row r="243" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>2296</v>
       </c>
@@ -23083,7 +23122,7 @@
       </c>
       <c r="V243" s="3"/>
     </row>
-    <row r="244" spans="1:23">
+    <row r="244" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>2306</v>
       </c>
@@ -23148,7 +23187,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="245" spans="1:23">
+    <row r="245" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>2315</v>
       </c>
@@ -23201,7 +23240,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="246" spans="1:23">
+    <row r="246" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>2323</v>
       </c>
@@ -23264,7 +23303,7 @@
       </c>
       <c r="V246" s="3"/>
     </row>
-    <row r="247" spans="1:23">
+    <row r="247" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>915</v>
       </c>
@@ -23330,7 +23369,7 @@
       </c>
       <c r="V247" s="3"/>
     </row>
-    <row r="248" spans="1:23">
+    <row r="248" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>2339</v>
       </c>
@@ -23393,7 +23432,7 @@
       </c>
       <c r="V248" s="3"/>
     </row>
-    <row r="249" spans="1:23">
+    <row r="249" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>2104</v>
       </c>
@@ -23459,7 +23498,7 @@
       </c>
       <c r="V249" s="3"/>
     </row>
-    <row r="250" spans="1:23">
+    <row r="250" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>1629</v>
       </c>
@@ -23518,7 +23557,7 @@
         <v>2359</v>
       </c>
     </row>
-    <row r="251" spans="1:23">
+    <row r="251" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>2360</v>
       </c>
@@ -23578,7 +23617,7 @@
       </c>
       <c r="V251" s="3"/>
     </row>
-    <row r="252" spans="1:23">
+    <row r="252" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>1898</v>
       </c>
@@ -23632,7 +23671,7 @@
       </c>
       <c r="V252" s="3"/>
     </row>
-    <row r="253" spans="1:23">
+    <row r="253" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>2373</v>
       </c>
@@ -23686,7 +23725,7 @@
       </c>
       <c r="V253" s="3"/>
     </row>
-    <row r="254" spans="1:23">
+    <row r="254" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>2377</v>
       </c>
@@ -23752,7 +23791,7 @@
       </c>
       <c r="V254" s="3"/>
     </row>
-    <row r="255" spans="1:23">
+    <row r="255" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>2388</v>
       </c>
@@ -23811,7 +23850,7 @@
         <v>2396</v>
       </c>
     </row>
-    <row r="256" spans="1:23">
+    <row r="256" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>2397</v>
       </c>
@@ -23868,7 +23907,7 @@
         <v>2405</v>
       </c>
     </row>
-    <row r="257" spans="1:23">
+    <row r="257" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>2406</v>
       </c>
@@ -23931,7 +23970,7 @@
       </c>
       <c r="U257" s="3"/>
     </row>
-    <row r="258" spans="1:23">
+    <row r="258" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>2416</v>
       </c>
@@ -23994,7 +24033,7 @@
       </c>
       <c r="U258" s="3"/>
     </row>
-    <row r="259" spans="1:23">
+    <row r="259" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>2045</v>
       </c>
@@ -24045,7 +24084,7 @@
       </c>
       <c r="U259" s="3"/>
     </row>
-    <row r="260" spans="1:23">
+    <row r="260" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>2431</v>
       </c>
@@ -24105,7 +24144,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="261" spans="1:23">
+    <row r="261" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>1841</v>
       </c>
@@ -24168,7 +24207,7 @@
       </c>
       <c r="U261" s="3"/>
     </row>
-    <row r="262" spans="1:23">
+    <row r="262" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>2446</v>
       </c>
@@ -24219,7 +24258,7 @@
       </c>
       <c r="U262" s="3"/>
     </row>
-    <row r="263" spans="1:23">
+    <row r="263" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>2453</v>
       </c>
@@ -24261,7 +24300,7 @@
         <v>2458</v>
       </c>
     </row>
-    <row r="264" spans="1:23">
+    <row r="264" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>2459</v>
       </c>
@@ -24318,7 +24357,7 @@
       </c>
       <c r="U264" s="3"/>
     </row>
-    <row r="265" spans="1:23">
+    <row r="265" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>2468</v>
       </c>
@@ -24381,7 +24420,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="266" spans="1:23">
+    <row r="266" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>1763</v>
       </c>
@@ -24438,7 +24477,7 @@
       </c>
       <c r="U266" s="3"/>
     </row>
-    <row r="267" spans="1:23">
+    <row r="267" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>2485</v>
       </c>
@@ -24498,7 +24537,7 @@
         <v>2494</v>
       </c>
     </row>
-    <row r="268" spans="1:23">
+    <row r="268" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>2495</v>
       </c>
@@ -24552,7 +24591,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="269" spans="1:23">
+    <row r="269" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>1746</v>
       </c>
@@ -24612,7 +24651,7 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="270" spans="1:23">
+    <row r="270" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>2509</v>
       </c>
@@ -24675,7 +24714,7 @@
       </c>
       <c r="U270" s="3"/>
     </row>
-    <row r="271" spans="1:23">
+    <row r="271" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>2517</v>
       </c>
@@ -24732,7 +24771,7 @@
       </c>
       <c r="U271" s="3"/>
     </row>
-    <row r="272" spans="1:23">
+    <row r="272" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>1865</v>
       </c>
@@ -24786,7 +24825,7 @@
         <v>2530</v>
       </c>
     </row>
-    <row r="273" spans="1:21">
+    <row r="273" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>2531</v>
       </c>
@@ -24843,7 +24882,7 @@
       </c>
       <c r="U273" s="3"/>
     </row>
-    <row r="274" spans="1:21">
+    <row r="274" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>2540</v>
       </c>
@@ -24900,7 +24939,7 @@
       </c>
       <c r="U274" s="3"/>
     </row>
-    <row r="275" spans="1:21">
+    <row r="275" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>2549</v>
       </c>
@@ -24963,7 +25002,7 @@
       </c>
       <c r="U275" s="3"/>
     </row>
-    <row r="276" spans="1:21">
+    <row r="276" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>2559</v>
       </c>
@@ -25023,7 +25062,7 @@
       </c>
       <c r="U276" s="3"/>
     </row>
-    <row r="277" spans="1:21">
+    <row r="277" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>2568</v>
       </c>
@@ -25086,7 +25125,7 @@
       </c>
       <c r="U277" s="3"/>
     </row>
-    <row r="278" spans="1:21">
+    <row r="278" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>2579</v>
       </c>
@@ -25137,7 +25176,7 @@
       </c>
       <c r="U278" s="3"/>
     </row>
-    <row r="279" spans="1:21">
+    <row r="279" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>2585</v>
       </c>
@@ -25197,7 +25236,7 @@
       </c>
       <c r="U279" s="3"/>
     </row>
-    <row r="280" spans="1:21">
+    <row r="280" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>2596</v>
       </c>
@@ -25257,7 +25296,7 @@
       </c>
       <c r="U280" s="3"/>
     </row>
-    <row r="281" spans="1:21">
+    <row r="281" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>893</v>
       </c>
@@ -25311,10 +25350,75 @@
       </c>
       <c r="U281" s="3"/>
     </row>
-    <row r="282" spans="1:21">
-      <c r="A282" s="4"/>
-    </row>
-    <row r="284" spans="1:21">
+    <row r="282" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A282" s="11"/>
+      <c r="B282" s="12" t="s">
+        <v>2614</v>
+      </c>
+      <c r="C282" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D282" s="12"/>
+      <c r="E282" s="12"/>
+      <c r="F282" s="12"/>
+      <c r="G282" s="6" t="s">
+        <v>2611</v>
+      </c>
+      <c r="H282" s="12"/>
+      <c r="I282" s="12"/>
+      <c r="J282" s="12"/>
+      <c r="K282" s="12"/>
+      <c r="L282" s="12"/>
+      <c r="M282" s="12"/>
+      <c r="N282" s="12"/>
+      <c r="O282" s="12"/>
+      <c r="P282" s="12"/>
+      <c r="Q282" s="12"/>
+      <c r="R282" s="12"/>
+      <c r="S282" s="12"/>
+      <c r="T282" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="X282" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="283" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A283" s="12"/>
+      <c r="B283" s="12" t="s">
+        <v>2615</v>
+      </c>
+      <c r="C283" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D283" s="12"/>
+      <c r="E283" s="12"/>
+      <c r="F283" s="12"/>
+      <c r="G283" s="12" t="s">
+        <v>2613</v>
+      </c>
+      <c r="H283" s="12"/>
+      <c r="I283" s="12"/>
+      <c r="J283" s="12"/>
+      <c r="K283" s="12"/>
+      <c r="L283" s="12"/>
+      <c r="M283" s="12"/>
+      <c r="N283" s="12"/>
+      <c r="O283" s="12"/>
+      <c r="P283" s="12"/>
+      <c r="Q283" s="12"/>
+      <c r="R283" s="12"/>
+      <c r="S283" s="13">
+        <v>37789241</v>
+      </c>
+      <c r="T283" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="X283" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="284" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="U284" s="4"/>
     </row>
   </sheetData>
@@ -25341,32 +25445,14 @@
     <hyperlink ref="G210" r:id="rId12" xr:uid="{9C6F312D-2D40-48BF-9DF8-13A5B7670B25}"/>
     <hyperlink ref="G231" r:id="rId13" xr:uid="{672E23F4-7C5C-474C-8704-F42E70C88DB8}"/>
     <hyperlink ref="G244" r:id="rId14" xr:uid="{BE5679E6-061D-48BB-BC1A-DB31C756F3CF}"/>
+    <hyperlink ref="G282" r:id="rId15" display="https://doi.org/10.1016/j.tcs.2018.10.026" xr:uid="{CE7ADE85-A8BC-424D-B955-6560DF7AEBBA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dcb3a164-bac8-4869-8890-79aed5dbbc1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C6D92F61CC0CFC4BB26F83E6D7B677B4" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3f1c7b4b5209f845053d600cd1174dc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dcb3a164-bac8-4869-8890-79aed5dbbc1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41dd85d039c7e72d1610d35d093f67ed" ns2:_="">
     <xsd:import namespace="dcb3a164-bac8-4869-8890-79aed5dbbc1d"/>
@@ -25544,14 +25630,57 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dcb3a164-bac8-4869-8890-79aed5dbbc1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57CBDBA6-31B9-458D-804A-75C10C6AAB8D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8A51923-ACE0-4F85-A240-9B48F6BE26C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dcb3a164-bac8-4869-8890-79aed5dbbc1d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63044C84-7690-42CF-B6B0-0228F3431266}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63044C84-7690-42CF-B6B0-0228F3431266}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8A51923-ACE0-4F85-A240-9B48F6BE26C7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57CBDBA6-31B9-458D-804A-75C10C6AAB8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dcb3a164-bac8-4869-8890-79aed5dbbc1d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>